<commit_message>
Adjusted some of the field sizes.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.6.xlsx
+++ b/schema_definitions/template_schema_v1.6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Desktop/__FUNNY__/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE43055-6189-BC40-842F-6B007AF3BFE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67418692-02E6-A047-B296-453C3CE77C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="12">
-        <v>255</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="R17" s="12">
-        <v>255</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1939,7 +1939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -2612,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="P1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2769,7 +2769,7 @@
         <v>96</v>
       </c>
       <c r="R3" s="7">
-        <v>255</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated format and contnet for country of recruitment
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.6.xlsx
+++ b/schema_definitions/template_schema_v1.6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Desktop/__FUNNY__/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Learning/CS224W/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67418692-02E6-A047-B296-453C3CE77C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF52103-F000-9C43-9CEC-AFD7F6D3E592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -589,10 +589,10 @@
     <t>MANDATORY-GCST</t>
   </si>
   <si>
-    <t>Afghanistan|Albania|Algeria|American Samoa|Andorra|Angola|Anguilla|Antigua and Barbuda|Argentina|Armenia|Australia|Austria|Azerbaijan|Bahamas|Bahrain|Bangladesh|Barbados|Belarus|Belgium|Belize|Benin|Bermuda|Bhutan|Bolivia|Bosnia and Herzegovina|Botswana|Brazil|British Virgin Islands|Brunei Darussalam|Bulgaria|Burkina Faso|Burundi|Cambodia|Cameroon|Canada|Cape Verde|Cayman Islands|Central African Republic|Chad|Channel Islands|Chile|China|China, Hong Kong SAR|China, Macao SAR|Colombia|Comoros|Congo|Cook Islands|Costa Rica|Croatia|Cuba|Cyprus|Cyprus|Czech Republic|Côte d’Ivoire|Democratic People’s Republic of Korea|Democratic Republic of the Congo|Denmark|Djibouti|Dominica|Dominican Republic|Ecuador|Egypt|El Salvador|Equatorial Guinea|Eritrea|Estonia|Ethiopia|Faeroe Islands|Falkland Islands (Malvinas)|Fiji|Finland|France|French Guiana|French Polynesia|Gabon|Gambia|Georgia|Germany|Ghana|Gibraltar|Greece|Greenland|Grenada|Guadeloupe|Guam|Guatemala|Guinea|Guinea-Bissau|Guyana|Haiti|Holy See|Honduras|Hungary|Iceland|India|Indonesia|Iran (Islamic Republic of)|Iraq|Isle of Man|Israel|Italy|Jamaica|Japan|Jordan|Kazakhstan|Kenya|Kiribati|Kuwait|Kyrgyzstan|Lao People’s Democratic Republic|Latvia|Lebanon|Lesotho|Liberia|Libyan Arab Jamahiriya|Liechtenstein|Lithuania|Luxembourg|Madagascar|Malawi|Malaysia|Maldives|Mali|Malta|Marshall Islands|Martinique|Mauretania|Mauritius|Mayotte|Mexico|Micronesia (Federated States of)|Monaco|Mongolia|Montenegro|Montserrat|Morocco|Mozambique|Myanmar|NR|Namibia|Nauru|Nepal|Netherlands|Netherlands Antilles|New Caledonia|New Zealand|Nicaragua|Niger|Nigeria|Niue|Norfolk Island|Norway|Occupied Palestinian Territory|Oman|Pakistan|Palau|Panama|Papua New Guinea|Paraguay|Peru|Philippines|Pitcairn|Poland|Portugal|Puerto Rico|Qatar|Republic of Ireland|Republic of Korea|Republic of Moldova|Romania|Russian Federation|Rwanda|Réunion|Saint Kitts and Nevis|Saint Lucia|Saint Vincent and the Grenadines|Saint-Pierre-et-Miquelon|Samoa|San Marino|Saudi Arabia|Senegal|Serbia|Seychelles|Sierra Leone|Singapore|Slovakia|Slovenia|Solomon Islands|Somalia|South Africa|Spain|Sri Lanka|St. Helena|Sudan|Suriname|Swaziland|Sweden|Switzerland|São Tomé and Príncipe|Taiwan|Tajikistan|Thailand|The former Yugoslav Republic of Macedonia|Timor-Leste|Togo|Tokelau|Tonga|Trinidad and Tobago|Tunisia|Turkey|Turkmenistan|Turks and Caicos Islands|Tuvalu|U.K.|U.S.|U.S. Virgin Islands|Uganda|Ukraine|United Arab Emirates|United Republic of Tanzania|Uruguay|Uzbekistan|Vanuatu|Venezuela|Viet Nam|Wallis and Futuna Islands|Western Sahara|Yemen|Zambia|Zimbabwe</t>
-  </si>
-  <si>
     <t>SIZE</t>
+  </si>
+  <si>
+    <t>Afghanistan|Albania|Algeria|American Samoa|Andorra|Angola|Anguilla|Antigua and Barbuda|Argentina|Armenia|Australia|Austria|Azerbaijan|Bahamas|Bahrain|Bangladesh|Barbados|Belarus|Belgium|Belize|Benin|Bermuda|Bhutan|Bolivia|Bosnia and Herzegovina|Botswana|Brazil|British Virgin Islands|Brunei Darussalam|Bulgaria|Burkina Faso|Burundi|Cambodia|Cameroon|Canada|Cape Verde|Cayman Islands|Central African Republic|Chad|Channel Islands|Chile|China|China, Hong Kong SAR|China, Macao SAR|Colombia|Comoros|Congo|Cook Islands|Costa Rica|Croatia|Cuba|Cyprus|Cyprus|Czech Republic|Côte d’Ivoire:Cote d’Ivoire|Democratic People’s Republic of Korea:North Korea|Democratic Republic of the Congo|Denmark|Djibouti|Dominica|Dominican Republic|Ecuador|Egypt|El Salvador|Equatorial Guinea|Eritrea|Estonia|Ethiopia|Faeroe Islands|Falkland Islands (Malvinas)|Fiji|Finland|France|French Guiana|French Polynesia|Gabon|Gambia|Georgia|Germany|Ghana|Gibraltar|Greece|Greenland|Grenada|Guadeloupe|Guam|Guatemala|Guinea|Guinea-Bissau|Guyana|Haiti|Holy See|Honduras|Hong Kong:China, Hong Kong SAR|Hungary|Iceland|India|Indonesia|Iran (Islamic Republic of):Iran|Iraq|Isle of Man|Israel|Italy|Jamaica|Japan|Jordan|Kazakhstan|Kenya|Kiribati|Kuwait|Kyrgyzstan|Lao People’s Democratic Republic|Latvia|Lebanon|Lesotho|Liberia|Libyan Arab Jamahiriya|Liechtenstein|Lithuania|Luxembourg|Madagascar|Malawi|Malaysia|Maldives|Mali|Malta|Marshall Islands|Martinique|Mauretania|Mauritius|Mayotte|Mexico|Micronesia (Federated States of)|Monaco|Mongolia|Montenegro|Montserrat|Morocco|Mozambique|Myanmar|NR|Namibia|Nauru|Nepal|Netherlands|Netherlands Antilles|New Caledonia|New Zealand|Nicaragua|Niger|Nigeria|Niue|Norfolk Island|Norway|Occupied Palestinian Territory|Oman|Pakistan|Palau|Panama|Papua New Guinea|Paraguay|Peru|Philippines|Pitcairn|Poland|Portugal|Puerto Rico|Qatar|Republic of Ireland|Republic of Korea:South Korea|Republic of Moldova|Romania|Russian Federation|Rwanda|Réunion:Reunion|Saint Kitts and Nevis|Saint Lucia|Saint Vincent and the Grenadines|Saint-Pierre-et-Miquelon|Samoa|San Marino|Saudi Arabia|Senegal|Serbia|Seychelles|Sierra Leone|Singapore|Slovakia|Slovenia|Solomon Islands|Somalia|South Africa|Spain|Sri Lanka|St. Helena|Sudan|Suriname|Swaziland|Sweden|Switzerland|São Tomé and Príncipe:Sao Tome and Principe|Taiwan|Tajikistan|Thailand|The former Yugoslav Republic of Macedonia|Timor-Leste|Togo|Tokelau|Tonga|Trinidad and Tobago|Tunisia|Turkey|Turkmenistan|Turks and Caicos Islands|Tuvalu|U.K.:UK;United Kingdom;Great Britain;Britain|U.S.:US;USA;United States|U.S. Virgin Islands|Uganda|Ukraine|United Arab Emirates|United Republic of Tanzania|Uruguay|Uzbekistan|Vanuatu|Venezuela|Viet Nam|Wallis and Futuna Islands|Western Sahara|Yemen|Zambia|Zimbabwe</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -1094,7 +1094,7 @@
         <v>9</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -2014,7 +2014,7 @@
         <v>9</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -2612,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2687,7 +2687,7 @@
         <v>9</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3093,7 +3093,7 @@
         <v>171</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="R11" s="7">
         <v>255</v>
@@ -4172,7 +4172,7 @@
         <v>9</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Removed 255 char size constraint on sample_description.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.6.xlsx
+++ b/schema_definitions/template_schema_v1.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Learning/CS224W/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Work/EBI/IMPORT_TEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF52103-F000-9C43-9CEC-AFD7F6D3E592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8499731-B0E3-3244-9585-CFE3573E5D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="12">
-        <v>255</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -2612,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added more countries as per Elliot's suggestion.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.6.xlsx
+++ b/schema_definitions/template_schema_v1.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Work/EBI/IMPORT_TEST/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Work/EBI/prod_videos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8499731-B0E3-3244-9585-CFE3573E5D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5741B9-697F-A84D-87FD-0A36B006B4BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
     <t>SIZE</t>
   </si>
   <si>
-    <t>Afghanistan|Albania|Algeria|American Samoa|Andorra|Angola|Anguilla|Antigua and Barbuda|Argentina|Armenia|Australia|Austria|Azerbaijan|Bahamas|Bahrain|Bangladesh|Barbados|Belarus|Belgium|Belize|Benin|Bermuda|Bhutan|Bolivia|Bosnia and Herzegovina|Botswana|Brazil|British Virgin Islands|Brunei Darussalam|Bulgaria|Burkina Faso|Burundi|Cambodia|Cameroon|Canada|Cape Verde|Cayman Islands|Central African Republic|Chad|Channel Islands|Chile|China|China, Hong Kong SAR|China, Macao SAR|Colombia|Comoros|Congo|Cook Islands|Costa Rica|Croatia|Cuba|Cyprus|Cyprus|Czech Republic|Côte d’Ivoire:Cote d’Ivoire|Democratic People’s Republic of Korea:North Korea|Democratic Republic of the Congo|Denmark|Djibouti|Dominica|Dominican Republic|Ecuador|Egypt|El Salvador|Equatorial Guinea|Eritrea|Estonia|Ethiopia|Faeroe Islands|Falkland Islands (Malvinas)|Fiji|Finland|France|French Guiana|French Polynesia|Gabon|Gambia|Georgia|Germany|Ghana|Gibraltar|Greece|Greenland|Grenada|Guadeloupe|Guam|Guatemala|Guinea|Guinea-Bissau|Guyana|Haiti|Holy See|Honduras|Hong Kong:China, Hong Kong SAR|Hungary|Iceland|India|Indonesia|Iran (Islamic Republic of):Iran|Iraq|Isle of Man|Israel|Italy|Jamaica|Japan|Jordan|Kazakhstan|Kenya|Kiribati|Kuwait|Kyrgyzstan|Lao People’s Democratic Republic|Latvia|Lebanon|Lesotho|Liberia|Libyan Arab Jamahiriya|Liechtenstein|Lithuania|Luxembourg|Madagascar|Malawi|Malaysia|Maldives|Mali|Malta|Marshall Islands|Martinique|Mauretania|Mauritius|Mayotte|Mexico|Micronesia (Federated States of)|Monaco|Mongolia|Montenegro|Montserrat|Morocco|Mozambique|Myanmar|NR|Namibia|Nauru|Nepal|Netherlands|Netherlands Antilles|New Caledonia|New Zealand|Nicaragua|Niger|Nigeria|Niue|Norfolk Island|Norway|Occupied Palestinian Territory|Oman|Pakistan|Palau|Panama|Papua New Guinea|Paraguay|Peru|Philippines|Pitcairn|Poland|Portugal|Puerto Rico|Qatar|Republic of Ireland|Republic of Korea:South Korea|Republic of Moldova|Romania|Russian Federation|Rwanda|Réunion:Reunion|Saint Kitts and Nevis|Saint Lucia|Saint Vincent and the Grenadines|Saint-Pierre-et-Miquelon|Samoa|San Marino|Saudi Arabia|Senegal|Serbia|Seychelles|Sierra Leone|Singapore|Slovakia|Slovenia|Solomon Islands|Somalia|South Africa|Spain|Sri Lanka|St. Helena|Sudan|Suriname|Swaziland|Sweden|Switzerland|São Tomé and Príncipe:Sao Tome and Principe|Taiwan|Tajikistan|Thailand|The former Yugoslav Republic of Macedonia|Timor-Leste|Togo|Tokelau|Tonga|Trinidad and Tobago|Tunisia|Turkey|Turkmenistan|Turks and Caicos Islands|Tuvalu|U.K.:UK;United Kingdom;Great Britain;Britain|U.S.:US;USA;United States|U.S. Virgin Islands|Uganda|Ukraine|United Arab Emirates|United Republic of Tanzania|Uruguay|Uzbekistan|Vanuatu|Venezuela|Viet Nam|Wallis and Futuna Islands|Western Sahara|Yemen|Zambia|Zimbabwe</t>
+    <t>Afghanistan|Albania|Algeria|American Samoa|Andorra|Angola|Anguilla|Antigua and Barbuda|Argentina|Armenia|Australia|Austria|Azerbaijan|Bahamas|Bahrain|Bangladesh|Barbados|Belarus|Belgium|Belize|Benin|Bermuda|Bhutan|Bolivia|Bosnia and Herzegovina|Botswana|Brazil|British Virgin Islands|Brunei Darussalam:Brunei|Bulgaria|Burkina Faso|Burundi|Cambodia|Cameroon|Canada|Cape Verde|Cayman Islands|Central African Republic|Chad|Channel Islands|Chile|China|China, Hong Kong SAR|China, Macao SAR:Macao;Macau|Colombia|Comoros|Congo|Cook Islands|Costa Rica|Croatia|Cuba|Cyprus|Cyprus|Czech Republic:Czechia|Côte d’Ivoire:Cote d’Ivoire;Ivory Coast|Democratic People’s Republic of Korea:North Korea|Democratic Republic of the Congo|Denmark|Djibouti|Dominica|Dominican Republic|Ecuador|Egypt|El Salvador|Equatorial Guinea|Eritrea|Estonia|Ethiopia|Faeroe Islands:Faroe Islands|Falkland Islands (Malvinas)|Fiji|Finland|France|French Guiana|French Polynesia|Gabon|Gambia|Georgia|Germany|Ghana|Gibraltar|Greece|Greenland|Grenada|Guadeloupe|Guam|Guatemala|Guinea|Guinea-Bissau|Guyana|Haiti|Holy See|Honduras|Hong Kong:China, Hong Kong SAR|Hungary|Iceland|India|Indonesia|Iran (Islamic Republic of):Iran|Iraq|Isle of Man|Israel|Italy|Jamaica|Japan|Jordan|Kazakhstan|Kenya|Kiribati|Kuwait|Kyrgyzstan|Lao People’s Democratic Republic:Laos|Latvia|Lebanon|Lesotho|Liberia|Libyan Arab Jamahiriya:Libya|Liechtenstein|Lithuania|Luxembourg|Madagascar|Malawi|Malaysia|Maldives|Mali|Malta|Marshall Islands|Martinique|Mauretania|Mauritius|Mayotte|Mexico|Micronesia (Federated States of):Micronesia;Federated States of Micronesia|Monaco|Mongolia|Montenegro|Montserrat|Morocco|Mozambique|Myanmar|NR|Namibia|Nauru|Nepal|Netherlands|Netherlands Antilles|New Caledonia|New Zealand|Nicaragua|Niger|Nigeria|Niue|Norfolk Island|Norway|Occupied Palestinian Territory:Palestine|Oman|Pakistan|Palau|Panama|Papua New Guinea|Paraguay|Peru|Philippines|Pitcairn|Poland|Portugal|Puerto Rico|Qatar|Republic of Ireland:Ireland|Republic of Korea:South Korea|Republic of Moldova:Moldova|Romania|Russian Federation:Russia|Rwanda|Réunion:Reunion|Saint Kitts and Nevis|Saint Lucia|Saint Vincent and the Grenadines|Saint-Pierre-et-Miquelon|Samoa|San Marino|Saudi Arabia|Senegal|Serbia|Seychelles|Sierra Leone|Singapore|Slovakia|Slovenia|Solomon Islands|Somalia|South Africa|South Sudan|Spain|Sri Lanka|St. Helena|Sudan|Suriname|Swaziland:Eswatini|Sweden|Switzerland|São Tomé and Príncipe:Sao Tome and Principe|Taiwan|Tajikistan|Thailand|The former Yugoslav Republic of Macedonia:North Macedonia|Timor-Leste|Togo|Tokelau|Tonga|Trinidad and Tobago|Tunisia|Turkey|Turkmenistan|Turks and Caicos Islands|Tuvalu|U.K.:UK;United Kingdom;Great Britain;Britain|U.S.:US;USA;United States|U.S. Virgin Islands:US Virgin Islands;United States Virgin Islands|Uganda|Ukraine|United Arab Emirates|United Republic of Tanzania:Tanzania|Uruguay|Uzbekistan|Vanuatu|Venezuela|Viet Nam:Vietnam|Wallis and Futuna Islands|Western Sahara|Yemen|Zambia|Zimbabwe</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
@@ -2612,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Removed size restriction on the readme field.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.6.xlsx
+++ b/schema_definitions/template_schema_v1.6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Work/EBI/prod_videos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Desktop/_GARETH_/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5741B9-697F-A84D-87FD-0A36B006B4BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7145BFF-7ECF-014C-A17E-3D0F2D93BE14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="R18" s="12">
-        <v>255</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -2612,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>